<commit_message>
adding setup functionality and working extraction
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\Development\nsbl-create-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C9C290-4E1B-4843-8CD8-AD735F3CFAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08161634-0513-4C28-AE0B-6BADD52B84D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31110" yWindow="2445" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="32775" yWindow="2370" windowWidth="21600" windowHeight="11385" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
     <sheet name="runsheet" sheetId="5" r:id="rId1"/>
@@ -91,24 +91,6 @@
     <t>_12_c1_</t>
   </si>
   <si>
-    <t>_13_c1_</t>
-  </si>
-  <si>
-    <t>_14_c1_</t>
-  </si>
-  <si>
-    <t>_15_c1_</t>
-  </si>
-  <si>
-    <t>_16_c1_</t>
-  </si>
-  <si>
-    <t>_17_c1_</t>
-  </si>
-  <si>
-    <t>_18_c1_</t>
-  </si>
-  <si>
     <t>_9_c2_</t>
   </si>
   <si>
@@ -121,24 +103,6 @@
     <t>_12_c2_</t>
   </si>
   <si>
-    <t>_13_c2_</t>
-  </si>
-  <si>
-    <t>_14_c2_</t>
-  </si>
-  <si>
-    <t>_15_c2_</t>
-  </si>
-  <si>
-    <t>_16_c2_</t>
-  </si>
-  <si>
-    <t>_17_c2_</t>
-  </si>
-  <si>
-    <t>_18_c2_</t>
-  </si>
-  <si>
     <t>WINNING TEAM:</t>
   </si>
   <si>
@@ -233,6 +197,42 @@
   </si>
   <si>
     <t>_b_player_name_</t>
+  </si>
+  <si>
+    <t>_1_c1_</t>
+  </si>
+  <si>
+    <t>_2_c1_</t>
+  </si>
+  <si>
+    <t>_3_c1_</t>
+  </si>
+  <si>
+    <t>_4_c1_</t>
+  </si>
+  <si>
+    <t>_5_c1_</t>
+  </si>
+  <si>
+    <t>_6_c1_</t>
+  </si>
+  <si>
+    <t>_1_c2_</t>
+  </si>
+  <si>
+    <t>_2_c2_</t>
+  </si>
+  <si>
+    <t>_3_c2_</t>
+  </si>
+  <si>
+    <t>_4_c2_</t>
+  </si>
+  <si>
+    <t>_5_c2_</t>
+  </si>
+  <si>
+    <t>_6_c2_</t>
   </si>
 </sst>
 </file>
@@ -1041,90 +1041,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1141,6 +1057,90 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1539,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06001A37-2C87-4F4D-8D59-4864FA219C19}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1593,7 +1593,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1608,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1623,7 +1623,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1631,14 +1631,14 @@
         <v>11</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1646,14 +1646,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1661,14 +1661,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1676,14 +1676,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1691,14 +1691,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -1706,14 +1706,14 @@
         <v>9</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1729,8 +1729,8 @@
   </sheetPr>
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Y1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1762,23 +1762,23 @@
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
       <c r="J1" s="57"/>
-      <c r="K1" s="89" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
+      <c r="K1" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
       <c r="Z1" s="56"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1787,24 +1787,24 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55"/>
-      <c r="K3" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="S3" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
+      <c r="K3" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="S3" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
       <c r="Z3" s="54"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -1818,25 +1818,25 @@
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
       <c r="J4" s="37"/>
-      <c r="K4" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
+      <c r="K4" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
       <c r="R4" s="38"/>
-      <c r="S4" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
+      <c r="S4" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
       <c r="Z4" s="52"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1850,23 +1850,23 @@
       <c r="H5" s="37"/>
       <c r="I5" s="37"/>
       <c r="J5" s="37"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="93" t="s">
-        <v>58</v>
-      </c>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="93"/>
+      <c r="S5" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
       <c r="Z5" s="52"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1880,25 +1880,25 @@
       <c r="H6" s="37"/>
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
-      <c r="K6" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
+      <c r="K6" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
       <c r="R6" s="38"/>
-      <c r="S6" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="94"/>
-      <c r="W6" s="94"/>
-      <c r="X6" s="94"/>
-      <c r="Y6" s="94"/>
+      <c r="S6" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="66"/>
       <c r="Z6" s="52"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1913,16 +1913,16 @@
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
       <c r="K7" s="38"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="65"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="69"/>
       <c r="P7" s="38"/>
-      <c r="Q7" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="R7" s="64"/>
-      <c r="S7" s="65"/>
+      <c r="Q7" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="68"/>
+      <c r="S7" s="69"/>
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
       <c r="V7" s="38"/>
@@ -1933,32 +1933,32 @@
     </row>
     <row r="8" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="71" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="72"/>
       <c r="D8" s="73" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E8" s="74"/>
       <c r="F8" s="74"/>
       <c r="G8" s="74"/>
       <c r="H8" s="74"/>
       <c r="I8" s="74"/>
-      <c r="J8" s="84"/>
+      <c r="J8" s="75"/>
       <c r="K8" s="38"/>
-      <c r="L8" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
+      <c r="L8" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
       <c r="P8" s="38"/>
-      <c r="Q8" s="85" t="s">
-        <v>52</v>
-      </c>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
+      <c r="Q8" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
       <c r="T8" s="38"/>
       <c r="U8" s="53"/>
       <c r="V8" s="38"/>
@@ -1968,45 +1968,45 @@
       <c r="Z8" s="52"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
+      <c r="A9" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="37"/>
-      <c r="E9" s="77" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="86" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
-      <c r="O9" s="87"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="87"/>
-      <c r="R9" s="87"/>
-      <c r="S9" s="87"/>
-      <c r="T9" s="87"/>
-      <c r="U9" s="87"/>
-      <c r="V9" s="87"/>
-      <c r="W9" s="87"/>
-      <c r="X9" s="87"/>
-      <c r="Y9" s="87"/>
-      <c r="Z9" s="88"/>
+      <c r="E9" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="82"/>
+      <c r="S9" s="82"/>
+      <c r="T9" s="82"/>
+      <c r="U9" s="82"/>
+      <c r="V9" s="82"/>
+      <c r="W9" s="82"/>
+      <c r="X9" s="82"/>
+      <c r="Y9" s="82"/>
+      <c r="Z9" s="83"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="B10" s="23"/>
       <c r="C10" s="37"/>
       <c r="D10" s="38" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="42">
@@ -2022,38 +2022,38 @@
         <v>4</v>
       </c>
       <c r="J10" s="37"/>
-      <c r="K10" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="81"/>
-      <c r="O10" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="81"/>
-      <c r="S10" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="T10" s="80"/>
-      <c r="U10" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="V10" s="81"/>
-      <c r="W10" s="79" t="s">
-        <v>36</v>
-      </c>
-      <c r="X10" s="80"/>
-      <c r="Y10" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z10" s="81"/>
+      <c r="K10" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="86"/>
+      <c r="O10" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="85"/>
+      <c r="Q10" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="86"/>
+      <c r="S10" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10" s="85"/>
+      <c r="U10" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="V10" s="86"/>
+      <c r="W10" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="85"/>
+      <c r="Y10" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z10" s="86"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39"/>
@@ -2112,7 +2112,7 @@
       <c r="B12" s="23"/>
       <c r="C12" s="37"/>
       <c r="D12" s="38" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="45">
@@ -2218,7 +2218,7 @@
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
@@ -2260,18 +2260,18 @@
       <c r="Z14" s="30"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="82"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="38"/>
       <c r="D15" s="37"/>
       <c r="E15" s="37"/>
-      <c r="F15" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
+      <c r="F15" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="31"/>
       <c r="L15" s="22">
         <v>5</v>
@@ -2306,15 +2306,15 @@
       <c r="Z15" s="30"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="70"/>
+      <c r="A16" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="90"/>
       <c r="F16" s="36">
         <v>1</v>
       </c>
@@ -2364,15 +2364,15 @@
       <c r="Z16" s="30"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="65"/>
+      <c r="A17" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="69"/>
       <c r="F17" s="33"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
@@ -2412,11 +2412,11 @@
       <c r="Z17" s="30"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="65"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="33"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
@@ -2456,11 +2456,11 @@
       <c r="Z18" s="30"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="65"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="33"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
@@ -2500,11 +2500,11 @@
       <c r="Z19" s="30"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="65"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="33"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
@@ -2544,11 +2544,11 @@
       <c r="Z20" s="30"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="65"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="33"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
@@ -2588,11 +2588,11 @@
       <c r="Z21" s="30"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="65"/>
+      <c r="A22" s="87"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="33"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
@@ -2632,11 +2632,11 @@
       <c r="Z22" s="30"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="65"/>
+      <c r="A23" s="87"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="33"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
@@ -2676,11 +2676,11 @@
       <c r="Z23" s="30"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="65"/>
+      <c r="A24" s="87"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="33"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
@@ -2720,11 +2720,11 @@
       <c r="Z24" s="30"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="65"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="33"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
@@ -2764,11 +2764,11 @@
       <c r="Z25" s="30"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="65"/>
+      <c r="A26" s="87"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="33"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
@@ -2808,11 +2808,11 @@
       <c r="Z26" s="30"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="65"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="33"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
@@ -2852,11 +2852,11 @@
       <c r="Z27" s="30"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="65"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="33"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
@@ -2897,12 +2897,12 @@
     </row>
     <row r="29" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="71" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B29" s="72"/>
       <c r="C29" s="72"/>
       <c r="D29" s="73" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E29" s="74"/>
       <c r="F29" s="74"/>
@@ -2944,20 +2944,20 @@
       <c r="Z29" s="30"/>
     </row>
     <row r="30" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
+      <c r="A30" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="37"/>
-      <c r="E30" s="77" t="s">
-        <v>48</v>
-      </c>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="78"/>
+      <c r="E30" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="31"/>
       <c r="L30" s="22">
         <v>20</v>
@@ -2996,7 +2996,7 @@
       <c r="B31" s="23"/>
       <c r="C31" s="37"/>
       <c r="D31" s="38" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E31" s="38"/>
       <c r="F31" s="42">
@@ -3102,7 +3102,7 @@
       <c r="B33" s="23"/>
       <c r="C33" s="37"/>
       <c r="D33" s="38" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E33" s="38"/>
       <c r="F33" s="45">
@@ -3208,7 +3208,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
@@ -3250,18 +3250,18 @@
       <c r="Z35" s="30"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
-      <c r="B36" s="68"/>
+      <c r="A36" s="87"/>
+      <c r="B36" s="91"/>
       <c r="C36" s="38"/>
       <c r="D36" s="37"/>
       <c r="E36" s="37"/>
-      <c r="F36" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
+      <c r="F36" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
       <c r="K36" s="31"/>
       <c r="L36" s="22">
         <v>26</v>
@@ -3296,15 +3296,15 @@
       <c r="Z36" s="30"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="64"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="70"/>
+      <c r="A37" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="68"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="90"/>
       <c r="F37" s="36">
         <v>1</v>
       </c>
@@ -3354,15 +3354,15 @@
       <c r="Z37" s="30"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="65"/>
+      <c r="A38" s="87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="68"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="69"/>
       <c r="F38" s="33"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23"/>
@@ -3402,11 +3402,11 @@
       <c r="Z38" s="30"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="63"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="65"/>
+      <c r="A39" s="87"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="33"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
@@ -3446,11 +3446,11 @@
       <c r="Z39" s="30"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="63"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="65"/>
+      <c r="A40" s="87"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="69"/>
       <c r="F40" s="33"/>
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
@@ -3490,11 +3490,11 @@
       <c r="Z40" s="30"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="65"/>
+      <c r="A41" s="87"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="33"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
@@ -3534,11 +3534,11 @@
       <c r="Z41" s="30"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="65"/>
+      <c r="A42" s="87"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="33"/>
       <c r="G42" s="23"/>
       <c r="H42" s="23"/>
@@ -3578,11 +3578,11 @@
       <c r="Z42" s="30"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="65"/>
+      <c r="A43" s="87"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="33"/>
       <c r="G43" s="23"/>
       <c r="H43" s="23"/>
@@ -3622,11 +3622,11 @@
       <c r="Z43" s="30"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="63"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="65"/>
+      <c r="A44" s="87"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="33"/>
       <c r="G44" s="23"/>
       <c r="H44" s="23"/>
@@ -3666,11 +3666,11 @@
       <c r="Z44" s="30"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="63"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="66"/>
-      <c r="E45" s="65"/>
+      <c r="A45" s="87"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="69"/>
       <c r="F45" s="33"/>
       <c r="G45" s="23"/>
       <c r="H45" s="23"/>
@@ -3710,11 +3710,11 @@
       <c r="Z45" s="30"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="63"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="65"/>
+      <c r="A46" s="87"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="69"/>
       <c r="F46" s="33"/>
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
@@ -3754,11 +3754,11 @@
       <c r="Z46" s="30"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="63"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="65"/>
+      <c r="A47" s="87"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="69"/>
       <c r="F47" s="33"/>
       <c r="G47" s="23"/>
       <c r="H47" s="23"/>
@@ -3798,11 +3798,11 @@
       <c r="Z47" s="30"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="63"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="65"/>
+      <c r="A48" s="87"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="33"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23"/>
@@ -3842,11 +3842,11 @@
       <c r="Z48" s="30"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="63"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="65"/>
+      <c r="A49" s="87"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="69"/>
       <c r="F49" s="33"/>
       <c r="G49" s="23"/>
       <c r="H49" s="23"/>
@@ -3887,11 +3887,11 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="29"/>
-      <c r="B50" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
+      <c r="B50" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="92"/>
+      <c r="D50" s="92"/>
       <c r="E50" s="29"/>
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
@@ -3933,21 +3933,21 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="24"/>
-      <c r="B51" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="61"/>
+      <c r="B51" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
       <c r="E51" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93"/>
       <c r="H51" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I51" s="61"/>
-      <c r="J51" s="61"/>
+        <v>23</v>
+      </c>
+      <c r="I51" s="93"/>
+      <c r="J51" s="93"/>
       <c r="K51" s="22"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
@@ -3967,78 +3967,78 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="23"/>
-      <c r="B52" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="61"/>
+      <c r="B52" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="93"/>
+      <c r="D52" s="93"/>
       <c r="E52" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="F52" s="93"/>
+      <c r="G52" s="93"/>
       <c r="H52" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I52" s="61"/>
-      <c r="J52" s="61"/>
+        <v>23</v>
+      </c>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
       <c r="K52" s="22"/>
-      <c r="L52" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="M52" s="62"/>
-      <c r="N52" s="62"/>
-      <c r="O52" s="62"/>
-      <c r="P52" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q52" s="61"/>
-      <c r="R52" s="61"/>
-      <c r="S52" s="61"/>
-      <c r="T52" s="61"/>
-      <c r="U52" s="61" t="s">
-        <v>38</v>
-      </c>
-      <c r="V52" s="61"/>
-      <c r="W52" s="61"/>
-      <c r="X52" s="61"/>
-      <c r="Y52" s="61"/>
+      <c r="L52" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="M52" s="94"/>
+      <c r="N52" s="94"/>
+      <c r="O52" s="94"/>
+      <c r="P52" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q52" s="93"/>
+      <c r="R52" s="93"/>
+      <c r="S52" s="93"/>
+      <c r="T52" s="93"/>
+      <c r="U52" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="V52" s="93"/>
+      <c r="W52" s="93"/>
+      <c r="X52" s="93"/>
+      <c r="Y52" s="93"/>
       <c r="Z52" s="22"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="23"/>
-      <c r="B53" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
+      <c r="B53" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="94"/>
+      <c r="D53" s="94"/>
       <c r="E53" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
+        <v>24</v>
+      </c>
+      <c r="F53" s="93"/>
+      <c r="G53" s="93"/>
       <c r="H53" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I53" s="61"/>
-      <c r="J53" s="61"/>
-      <c r="K53" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="L53" s="62"/>
-      <c r="M53" s="62"/>
-      <c r="N53" s="62"/>
-      <c r="O53" s="62"/>
-      <c r="P53" s="62"/>
-      <c r="Q53" s="62"/>
-      <c r="R53" s="61"/>
-      <c r="S53" s="61"/>
-      <c r="T53" s="61"/>
-      <c r="U53" s="61"/>
-      <c r="V53" s="61"/>
-      <c r="W53" s="61"/>
-      <c r="X53" s="61"/>
-      <c r="Y53" s="61"/>
+        <v>23</v>
+      </c>
+      <c r="I53" s="93"/>
+      <c r="J53" s="93"/>
+      <c r="K53" s="94" t="s">
+        <v>22</v>
+      </c>
+      <c r="L53" s="94"/>
+      <c r="M53" s="94"/>
+      <c r="N53" s="94"/>
+      <c r="O53" s="94"/>
+      <c r="P53" s="94"/>
+      <c r="Q53" s="94"/>
+      <c r="R53" s="93"/>
+      <c r="S53" s="93"/>
+      <c r="T53" s="93"/>
+      <c r="U53" s="93"/>
+      <c r="V53" s="93"/>
+      <c r="W53" s="93"/>
+      <c r="X53" s="93"/>
+      <c r="Y53" s="93"/>
       <c r="Z53" s="22"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
@@ -4170,93 +4170,6 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B50:D50"/>
     <mergeCell ref="U52:W52"/>
     <mergeCell ref="X52:Y52"/>
     <mergeCell ref="B53:D53"/>
@@ -4273,6 +4186,93 @@
     <mergeCell ref="L52:O52"/>
     <mergeCell ref="P52:R52"/>
     <mergeCell ref="S52:T52"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
   </mergeCells>
   <pageMargins left="0.47" right="0.36" top="0.47" bottom="0.21" header="0.2" footer="0.21"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>